<commit_message>
Change labels of data, as well as adjusting the pixel size of the labels so it doesn't spill over in the boxes
</commit_message>
<xml_diff>
--- a/R/practice/shiny/chatgpt-forecaster-demo/data.xlsx
+++ b/R/practice/shiny/chatgpt-forecaster-demo/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpark\Documents\Development\Personal\learning\R\practice\shiny\chatgpt-forecaster-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6E0132-DBCB-4B50-97B1-B8552AB93D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500C5041-0F2D-4E11-BFE7-6054169979EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,13 +86,13 @@
     <t>AD-SPEND</t>
   </si>
   <si>
-    <t>AD-CREATIVITY</t>
-  </si>
-  <si>
     <t>PRODUCT-LAUNCH</t>
   </si>
   <si>
-    <t>MEDIA-EFFECT</t>
+    <t>CREATIVE-SCORE</t>
+  </si>
+  <si>
+    <t>MEDIA-MIX</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:I4577"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A470" workbookViewId="0">
-      <selection activeCell="H477" sqref="H477"/>
+      <selection activeCell="B484" sqref="B484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>44197</v>
@@ -701,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>44197</v>
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1">
         <v>44228</v>
@@ -1021,7 +1021,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
         <v>44228</v>
@@ -1149,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1">
         <v>44256</v>
@@ -1341,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1">
         <v>44256</v>
@@ -1469,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1">
         <v>44287</v>
@@ -1661,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1">
         <v>44287</v>
@@ -1789,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C43" s="1">
         <v>44317</v>
@@ -1981,7 +1981,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1">
         <v>44317</v>
@@ -2109,7 +2109,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C53" s="1">
         <v>44348</v>
@@ -2301,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" s="1">
         <v>44348</v>
@@ -2429,7 +2429,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C63" s="1">
         <v>44378</v>
@@ -2621,7 +2621,7 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C69" s="1">
         <v>44378</v>
@@ -2749,7 +2749,7 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C73" s="1">
         <v>44409</v>
@@ -2941,7 +2941,7 @@
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C79" s="1">
         <v>44409</v>
@@ -3069,7 +3069,7 @@
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C83" s="1">
         <v>44440</v>
@@ -3261,7 +3261,7 @@
         <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C89" s="1">
         <v>44440</v>
@@ -3389,7 +3389,7 @@
         <v>3</v>
       </c>
       <c r="B93" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C93" s="1">
         <v>44470</v>
@@ -3581,7 +3581,7 @@
         <v>3</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C99" s="1">
         <v>44470</v>
@@ -3709,7 +3709,7 @@
         <v>3</v>
       </c>
       <c r="B103" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C103" s="1">
         <v>44501</v>
@@ -3901,7 +3901,7 @@
         <v>3</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C109" s="1">
         <v>44501</v>
@@ -4029,7 +4029,7 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C113" s="1">
         <v>44531</v>
@@ -4221,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="B119" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C119" s="1">
         <v>44531</v>
@@ -4349,7 +4349,7 @@
         <v>3</v>
       </c>
       <c r="B123" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C123" s="1">
         <v>44562</v>
@@ -4541,7 +4541,7 @@
         <v>3</v>
       </c>
       <c r="B129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C129" s="1">
         <v>44562</v>
@@ -4669,7 +4669,7 @@
         <v>3</v>
       </c>
       <c r="B133" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C133" s="1">
         <v>44593</v>
@@ -4861,7 +4861,7 @@
         <v>3</v>
       </c>
       <c r="B139" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C139" s="1">
         <v>44593</v>
@@ -4989,7 +4989,7 @@
         <v>3</v>
       </c>
       <c r="B143" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C143" s="1">
         <v>44621</v>
@@ -5181,7 +5181,7 @@
         <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C149" s="1">
         <v>44621</v>
@@ -5309,7 +5309,7 @@
         <v>3</v>
       </c>
       <c r="B153" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C153" s="1">
         <v>44652</v>
@@ -5501,7 +5501,7 @@
         <v>3</v>
       </c>
       <c r="B159" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C159" s="1">
         <v>44652</v>
@@ -5629,7 +5629,7 @@
         <v>3</v>
       </c>
       <c r="B163" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C163" s="1">
         <v>44682</v>
@@ -5821,7 +5821,7 @@
         <v>3</v>
       </c>
       <c r="B169" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C169" s="1">
         <v>44682</v>
@@ -5949,7 +5949,7 @@
         <v>3</v>
       </c>
       <c r="B173" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C173" s="1">
         <v>44713</v>
@@ -6141,7 +6141,7 @@
         <v>3</v>
       </c>
       <c r="B179" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C179" s="1">
         <v>44713</v>
@@ -6269,7 +6269,7 @@
         <v>3</v>
       </c>
       <c r="B183" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C183" s="1">
         <v>44743</v>
@@ -6461,7 +6461,7 @@
         <v>3</v>
       </c>
       <c r="B189" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C189" s="1">
         <v>44743</v>
@@ -6589,7 +6589,7 @@
         <v>3</v>
       </c>
       <c r="B193" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C193" s="1">
         <v>44774</v>
@@ -6781,7 +6781,7 @@
         <v>3</v>
       </c>
       <c r="B199" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C199" s="1">
         <v>44774</v>
@@ -6909,7 +6909,7 @@
         <v>3</v>
       </c>
       <c r="B203" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C203" s="1">
         <v>44805</v>
@@ -7101,7 +7101,7 @@
         <v>3</v>
       </c>
       <c r="B209" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C209" s="1">
         <v>44805</v>
@@ -7229,7 +7229,7 @@
         <v>3</v>
       </c>
       <c r="B213" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C213" s="1">
         <v>44835</v>
@@ -7421,7 +7421,7 @@
         <v>3</v>
       </c>
       <c r="B219" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C219" s="1">
         <v>44835</v>
@@ -7549,7 +7549,7 @@
         <v>3</v>
       </c>
       <c r="B223" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C223" s="1">
         <v>44866</v>
@@ -7741,7 +7741,7 @@
         <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C229" s="1">
         <v>44866</v>
@@ -7869,7 +7869,7 @@
         <v>3</v>
       </c>
       <c r="B233" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C233" s="1">
         <v>44896</v>
@@ -8061,7 +8061,7 @@
         <v>3</v>
       </c>
       <c r="B239" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C239" s="1">
         <v>44896</v>
@@ -8189,7 +8189,7 @@
         <v>3</v>
       </c>
       <c r="B243" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C243" s="1">
         <v>44927</v>
@@ -8381,7 +8381,7 @@
         <v>3</v>
       </c>
       <c r="B249" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C249" s="1">
         <v>44927</v>
@@ -8509,7 +8509,7 @@
         <v>3</v>
       </c>
       <c r="B253" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C253" s="1">
         <v>44958</v>
@@ -8701,7 +8701,7 @@
         <v>3</v>
       </c>
       <c r="B259" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C259" s="1">
         <v>44958</v>
@@ -8829,7 +8829,7 @@
         <v>3</v>
       </c>
       <c r="B263" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C263" s="1">
         <v>44986</v>
@@ -9021,7 +9021,7 @@
         <v>3</v>
       </c>
       <c r="B269" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C269" s="1">
         <v>44986</v>
@@ -9149,7 +9149,7 @@
         <v>3</v>
       </c>
       <c r="B273" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C273" s="1">
         <v>45017</v>
@@ -9341,7 +9341,7 @@
         <v>3</v>
       </c>
       <c r="B279" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C279" s="1">
         <v>45017</v>
@@ -9469,7 +9469,7 @@
         <v>3</v>
       </c>
       <c r="B283" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C283" s="1">
         <v>45047</v>
@@ -9661,7 +9661,7 @@
         <v>3</v>
       </c>
       <c r="B289" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C289" s="1">
         <v>45047</v>
@@ -9789,7 +9789,7 @@
         <v>3</v>
       </c>
       <c r="B293" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C293" s="1">
         <v>45078</v>
@@ -9981,7 +9981,7 @@
         <v>3</v>
       </c>
       <c r="B299" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C299" s="1">
         <v>45078</v>
@@ -10109,7 +10109,7 @@
         <v>3</v>
       </c>
       <c r="B303" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C303" s="1">
         <v>45108</v>
@@ -10301,7 +10301,7 @@
         <v>3</v>
       </c>
       <c r="B309" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C309" s="1">
         <v>45108</v>
@@ -10429,7 +10429,7 @@
         <v>3</v>
       </c>
       <c r="B313" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C313" s="1">
         <v>45139</v>
@@ -10621,7 +10621,7 @@
         <v>3</v>
       </c>
       <c r="B319" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C319" s="1">
         <v>45139</v>
@@ -10749,7 +10749,7 @@
         <v>3</v>
       </c>
       <c r="B323" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C323" s="1">
         <v>45170</v>
@@ -10941,7 +10941,7 @@
         <v>3</v>
       </c>
       <c r="B329" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C329" s="1">
         <v>45170</v>
@@ -11069,7 +11069,7 @@
         <v>3</v>
       </c>
       <c r="B333" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C333" s="1">
         <v>45200</v>
@@ -11261,7 +11261,7 @@
         <v>3</v>
       </c>
       <c r="B339" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C339" s="1">
         <v>45200</v>
@@ -11389,7 +11389,7 @@
         <v>3</v>
       </c>
       <c r="B343" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C343" s="1">
         <v>45231</v>
@@ -11581,7 +11581,7 @@
         <v>3</v>
       </c>
       <c r="B349" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C349" s="1">
         <v>45231</v>
@@ -11709,7 +11709,7 @@
         <v>3</v>
       </c>
       <c r="B353" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C353" s="1">
         <v>45261</v>
@@ -11901,7 +11901,7 @@
         <v>3</v>
       </c>
       <c r="B359" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C359" s="1">
         <v>45261</v>
@@ -12029,7 +12029,7 @@
         <v>3</v>
       </c>
       <c r="B363" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C363" s="1">
         <v>45292</v>
@@ -12221,7 +12221,7 @@
         <v>3</v>
       </c>
       <c r="B369" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C369" s="1">
         <v>45292</v>
@@ -12349,7 +12349,7 @@
         <v>3</v>
       </c>
       <c r="B373" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C373" s="1">
         <v>45323</v>
@@ -12541,7 +12541,7 @@
         <v>3</v>
       </c>
       <c r="B379" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C379" s="1">
         <v>45323</v>
@@ -12669,7 +12669,7 @@
         <v>3</v>
       </c>
       <c r="B383" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C383" s="1">
         <v>45352</v>
@@ -12861,7 +12861,7 @@
         <v>3</v>
       </c>
       <c r="B389" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C389" s="1">
         <v>45352</v>
@@ -12989,7 +12989,7 @@
         <v>3</v>
       </c>
       <c r="B393" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C393" s="1">
         <v>45383</v>
@@ -13181,7 +13181,7 @@
         <v>3</v>
       </c>
       <c r="B399" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C399" s="1">
         <v>45383</v>
@@ -13309,7 +13309,7 @@
         <v>3</v>
       </c>
       <c r="B403" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C403" s="1">
         <v>45413</v>
@@ -13501,7 +13501,7 @@
         <v>3</v>
       </c>
       <c r="B409" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C409" s="1">
         <v>45413</v>
@@ -13629,7 +13629,7 @@
         <v>3</v>
       </c>
       <c r="B413" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C413" s="1">
         <v>45444</v>
@@ -13821,7 +13821,7 @@
         <v>3</v>
       </c>
       <c r="B419" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C419" s="1">
         <v>45444</v>
@@ -13949,7 +13949,7 @@
         <v>3</v>
       </c>
       <c r="B423" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C423" s="1">
         <v>45474</v>
@@ -14141,7 +14141,7 @@
         <v>3</v>
       </c>
       <c r="B429" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C429" s="1">
         <v>45474</v>
@@ -14269,7 +14269,7 @@
         <v>3</v>
       </c>
       <c r="B433" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C433" s="1">
         <v>45505</v>
@@ -14461,7 +14461,7 @@
         <v>3</v>
       </c>
       <c r="B439" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C439" s="1">
         <v>45505</v>
@@ -14589,7 +14589,7 @@
         <v>3</v>
       </c>
       <c r="B443" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C443" s="1">
         <v>45536</v>
@@ -14781,7 +14781,7 @@
         <v>3</v>
       </c>
       <c r="B449" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C449" s="1">
         <v>45536</v>
@@ -14909,7 +14909,7 @@
         <v>3</v>
       </c>
       <c r="B453" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C453" s="1">
         <v>45566</v>
@@ -15101,7 +15101,7 @@
         <v>3</v>
       </c>
       <c r="B459" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C459" s="1">
         <v>45566</v>
@@ -15229,7 +15229,7 @@
         <v>3</v>
       </c>
       <c r="B463" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C463" s="1">
         <v>45597</v>
@@ -15421,7 +15421,7 @@
         <v>3</v>
       </c>
       <c r="B469" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C469" s="1">
         <v>45597</v>
@@ -15549,7 +15549,7 @@
         <v>3</v>
       </c>
       <c r="B473" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C473" s="1">
         <v>45627</v>
@@ -15741,7 +15741,7 @@
         <v>3</v>
       </c>
       <c r="B479" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C479" s="1">
         <v>45627</v>
@@ -15869,7 +15869,7 @@
         <v>3</v>
       </c>
       <c r="B483" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C483" s="1">
         <v>45658</v>
@@ -16061,7 +16061,7 @@
         <v>3</v>
       </c>
       <c r="B489" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C489" s="1">
         <v>45658</v>

</xml_diff>

<commit_message>
Incorporate Toms new chart and new data
</commit_message>
<xml_diff>
--- a/R/practice/shiny/chatgpt-forecaster-demo/data.xlsx
+++ b/R/practice/shiny/chatgpt-forecaster-demo/data.xlsx
@@ -5,30 +5,17 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpark\Documents\Development\Personal\learning\R\practice\shiny\chatgpt-forecaster-demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Russell\Desktop\BrightblueMM\git repos\foreasting_tool_clarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500C5041-0F2D-4E11-BFE7-6054169979EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BF26DB-3E5B-49E7-AE03-F176680A7E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2085" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -430,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E0704A-EBC0-467D-A22F-AB397E4D9AA8}">
   <dimension ref="A1:I4577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A470" workbookViewId="0">
-      <selection activeCell="B484" sqref="B484"/>
+    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
+      <selection activeCell="D482" sqref="D482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10723,25 +10710,25 @@
         <v>45170</v>
       </c>
       <c r="D322">
-        <v>4538.8670391394598</v>
+        <v>0</v>
       </c>
       <c r="E322">
         <v>1</v>
       </c>
       <c r="F322" s="2">
         <f t="shared" si="12"/>
-        <v>4538.8670391394598</v>
+        <v>0</v>
       </c>
       <c r="G322">
         <f t="shared" si="13"/>
-        <v>4538.8670391394598</v>
+        <v>0</v>
       </c>
       <c r="H322">
         <v>1</v>
       </c>
       <c r="I322" s="2">
         <f t="shared" si="14"/>
-        <v>4538.8670391394598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.35">
@@ -11043,25 +11030,25 @@
         <v>45200</v>
       </c>
       <c r="D332">
-        <v>4342.1221598334623</v>
+        <v>0</v>
       </c>
       <c r="E332">
         <v>1</v>
       </c>
       <c r="F332" s="2">
         <f t="shared" si="15"/>
-        <v>4342.1221598334623</v>
+        <v>0</v>
       </c>
       <c r="G332">
         <f t="shared" si="16"/>
-        <v>4342.1221598334623</v>
+        <v>0</v>
       </c>
       <c r="H332">
         <v>1</v>
       </c>
       <c r="I332" s="2">
         <f t="shared" si="17"/>
-        <v>4342.1221598334623</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.35">
@@ -11363,25 +11350,25 @@
         <v>45231</v>
       </c>
       <c r="D342">
-        <v>6047.6231603023107</v>
+        <v>2000</v>
       </c>
       <c r="E342">
         <v>1</v>
       </c>
       <c r="F342" s="2">
         <f t="shared" si="15"/>
-        <v>6047.6231603023107</v>
+        <v>2000</v>
       </c>
       <c r="G342">
         <f t="shared" si="16"/>
-        <v>6047.6231603023107</v>
+        <v>2000</v>
       </c>
       <c r="H342">
         <v>1</v>
       </c>
       <c r="I342" s="2">
         <f t="shared" si="17"/>
-        <v>6047.6231603023107</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.35">
@@ -11683,25 +11670,25 @@
         <v>45261</v>
       </c>
       <c r="D352">
-        <v>4790.1309355004196</v>
+        <v>0</v>
       </c>
       <c r="E352">
         <v>1</v>
       </c>
       <c r="F352" s="2">
         <f t="shared" si="15"/>
-        <v>4790.1309355004196</v>
+        <v>0</v>
       </c>
       <c r="G352">
         <f t="shared" si="16"/>
-        <v>4790.1309355004196</v>
+        <v>0</v>
       </c>
       <c r="H352">
         <v>1</v>
       </c>
       <c r="I352" s="2">
         <f t="shared" si="17"/>
-        <v>4790.1309355004196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.35">
@@ -12003,25 +11990,25 @@
         <v>45292</v>
       </c>
       <c r="D362">
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
       <c r="E362">
         <v>1</v>
       </c>
       <c r="F362" s="2">
         <f t="shared" si="15"/>
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
       <c r="G362">
         <f t="shared" si="16"/>
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
       <c r="H362">
         <v>1</v>
       </c>
       <c r="I362" s="2">
         <f t="shared" si="17"/>
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.35">
@@ -12323,25 +12310,25 @@
         <v>45323</v>
       </c>
       <c r="D372">
-        <v>4449.7913680140182</v>
+        <v>1000</v>
       </c>
       <c r="E372">
         <v>1</v>
       </c>
       <c r="F372" s="2">
         <f t="shared" si="15"/>
-        <v>4449.7913680140182</v>
+        <v>1000</v>
       </c>
       <c r="G372">
         <f t="shared" si="16"/>
-        <v>4449.7913680140182</v>
+        <v>1000</v>
       </c>
       <c r="H372">
         <v>1</v>
       </c>
       <c r="I372" s="2">
         <f t="shared" si="17"/>
-        <v>4449.7913680140182</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="373" spans="1:9" x14ac:dyDescent="0.35">
@@ -12643,25 +12630,25 @@
         <v>45352</v>
       </c>
       <c r="D382">
-        <v>4172.9469177316469</v>
+        <v>3000</v>
       </c>
       <c r="E382">
         <v>1</v>
       </c>
       <c r="F382" s="2">
         <f t="shared" si="15"/>
-        <v>4172.9469177316469</v>
+        <v>3000</v>
       </c>
       <c r="G382">
         <f t="shared" si="16"/>
-        <v>4172.9469177316469</v>
+        <v>3000</v>
       </c>
       <c r="H382">
         <v>1</v>
       </c>
       <c r="I382" s="2">
         <f t="shared" si="17"/>
-        <v>4172.9469177316469</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.35">
@@ -13283,25 +13270,25 @@
         <v>45413</v>
       </c>
       <c r="D402">
-        <v>4981.171443334274</v>
+        <v>7000</v>
       </c>
       <c r="E402">
         <v>1</v>
       </c>
       <c r="F402" s="2">
         <f t="shared" si="21"/>
-        <v>4981.171443334274</v>
+        <v>7000</v>
       </c>
       <c r="G402">
         <f t="shared" si="22"/>
-        <v>4981.171443334274</v>
+        <v>7000</v>
       </c>
       <c r="H402">
         <v>1</v>
       </c>
       <c r="I402" s="2">
         <f t="shared" si="23"/>
-        <v>4981.171443334274</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.35">
@@ -14243,25 +14230,25 @@
         <v>45505</v>
       </c>
       <c r="D432">
-        <v>5281.7337756510733</v>
+        <v>7000</v>
       </c>
       <c r="E432">
         <v>1</v>
       </c>
       <c r="F432" s="2">
         <f t="shared" si="21"/>
-        <v>5281.7337756510733</v>
+        <v>7000</v>
       </c>
       <c r="G432">
         <f t="shared" si="22"/>
-        <v>5281.7337756510733</v>
+        <v>7000</v>
       </c>
       <c r="H432">
         <v>1</v>
       </c>
       <c r="I432" s="2">
         <f t="shared" si="23"/>
-        <v>5281.7337756510733</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="433" spans="1:9" x14ac:dyDescent="0.35">
@@ -14883,25 +14870,25 @@
         <v>45566</v>
       </c>
       <c r="D452">
-        <v>5487.6208312952986</v>
+        <v>3000</v>
       </c>
       <c r="E452">
         <v>1</v>
       </c>
       <c r="F452" s="2">
         <f t="shared" si="21"/>
-        <v>5487.6208312952986</v>
+        <v>3000</v>
       </c>
       <c r="G452">
         <f t="shared" si="22"/>
-        <v>5487.6208312952986</v>
+        <v>3000</v>
       </c>
       <c r="H452">
         <v>1</v>
       </c>
       <c r="I452" s="2">
         <f t="shared" si="23"/>
-        <v>5487.6208312952986</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="453" spans="1:9" x14ac:dyDescent="0.35">
@@ -15203,25 +15190,25 @@
         <v>45597</v>
       </c>
       <c r="D462">
-        <v>4886.9552721148475</v>
+        <v>2000</v>
       </c>
       <c r="E462">
         <v>1</v>
       </c>
       <c r="F462" s="2">
         <f t="shared" si="24"/>
-        <v>4886.9552721148475</v>
+        <v>2000</v>
       </c>
       <c r="G462">
         <f t="shared" si="25"/>
-        <v>4886.9552721148475</v>
+        <v>2000</v>
       </c>
       <c r="H462">
         <v>1</v>
       </c>
       <c r="I462" s="2">
         <f t="shared" si="26"/>
-        <v>4886.9552721148475</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="463" spans="1:9" x14ac:dyDescent="0.35">
@@ -15523,25 +15510,25 @@
         <v>45627</v>
       </c>
       <c r="D472">
-        <v>4783.2830687757478</v>
+        <v>0</v>
       </c>
       <c r="E472">
         <v>1</v>
       </c>
       <c r="F472" s="2">
         <f t="shared" si="24"/>
-        <v>4783.2830687757478</v>
+        <v>0</v>
       </c>
       <c r="G472">
         <f t="shared" si="25"/>
-        <v>4783.2830687757478</v>
+        <v>0</v>
       </c>
       <c r="H472">
         <v>1</v>
       </c>
       <c r="I472" s="2">
         <f t="shared" si="26"/>
-        <v>4783.2830687757478</v>
+        <v>0</v>
       </c>
     </row>
     <row r="473" spans="1:9" x14ac:dyDescent="0.35">
@@ -15843,25 +15830,25 @@
         <v>45658</v>
       </c>
       <c r="D482">
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
       <c r="E482">
         <v>1</v>
       </c>
       <c r="F482" s="2">
         <f t="shared" si="24"/>
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
       <c r="G482">
         <f t="shared" si="25"/>
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
       <c r="H482">
         <v>1</v>
       </c>
       <c r="I482" s="2">
         <f t="shared" si="26"/>
-        <v>3474.7698148077675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="483" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>